<commit_message>
Re-upload due to uinit correction
</commit_message>
<xml_diff>
--- a/MYb11-mediated-protection_Fig3_data_growth-in-competition_24h.xlsx
+++ b/MYb11-mediated-protection_Fig3_data_growth-in-competition_24h.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nancy\Documents\Post-Doc\Research\MYb11-mediated protection\MYb11-mediated-protection\inhibition_in-vitro_Bt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OBENGN\Documents\Nancy\Papers\Kemlein_MT-protection\1_manuscript_maintenance of protection\github\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7065631C-F310-49FD-B954-277501CC9DE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01624AA3-E347-4F9F-BD23-12EDB272F73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5616" xr2:uid="{FB657766-886A-44CC-B294-4FA2636B168B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FB657766-886A-44CC-B294-4FA2636B168B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -137,9 +148,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -177,7 +188,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -283,7 +294,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -425,7 +436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CB2E60-7C95-4CA6-BB59-B09DAC8C8E2E}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,10 +486,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>91.570777777777806</v>
+        <v>9.157077777777781</v>
       </c>
       <c r="E2">
-        <v>15.839777777777799</v>
+        <v>1.5839777777777799</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -498,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>92.183444444444405</v>
+        <v>9.2183444444444405</v>
       </c>
       <c r="E3">
-        <v>16.452444444444499</v>
+        <v>1.6452444444444498</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -521,10 +532,10 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>101.192333333333</v>
+        <v>10.1192333333333</v>
       </c>
       <c r="E4">
-        <v>25.4613333333333</v>
+        <v>2.54613333333333</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -544,10 +555,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>87.770222222222202</v>
+        <v>8.7770222222222198</v>
       </c>
       <c r="E5">
-        <v>6.9192222222222197</v>
+        <v>0.69192222222222199</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -567,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>88.462000000000003</v>
+        <v>8.8461999999999996</v>
       </c>
       <c r="E6">
-        <v>7.6109999999999998</v>
+        <v>0.7611</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -590,10 +601,10 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>86.98</v>
+        <v>8.6980000000000004</v>
       </c>
       <c r="E7">
-        <v>6.1289999999999996</v>
+        <v>0.6129</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -613,10 +624,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>92.5625</v>
+        <v>9.2562499999999996</v>
       </c>
       <c r="E8">
-        <v>16.831499999999998</v>
+        <v>1.6831499999999999</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -636,10 +647,10 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>88.046499999999995</v>
+        <v>8.8046499999999988</v>
       </c>
       <c r="E9">
-        <v>12.3155</v>
+        <v>1.2315499999999999</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -659,10 +670,10 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>86.33</v>
+        <v>8.6329999999999991</v>
       </c>
       <c r="E10">
-        <v>10.599</v>
+        <v>1.0599000000000001</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -682,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>83.626000000000005</v>
+        <v>8.3626000000000005</v>
       </c>
       <c r="E11">
-        <v>2.7750000000000101</v>
+        <v>0.27750000000000102</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -705,10 +716,10 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>85.408500000000004</v>
+        <v>8.5408500000000007</v>
       </c>
       <c r="E12">
-        <v>4.5575000000000001</v>
+        <v>0.45574999999999999</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -728,10 +739,10 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>82.784499999999994</v>
+        <v>8.2784499999999994</v>
       </c>
       <c r="E13">
-        <v>1.93350000000001</v>
+        <v>0.19335000000000099</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -751,10 +762,10 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>116.27849999999999</v>
+        <v>11.627849999999999</v>
       </c>
       <c r="E14">
-        <v>40.547499999999999</v>
+        <v>4.0547500000000003</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -774,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>107.4875</v>
+        <v>10.748749999999999</v>
       </c>
       <c r="E15">
-        <v>31.756499999999999</v>
+        <v>3.1756500000000001</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -797,10 +808,10 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>103.15900000000001</v>
+        <v>10.315900000000001</v>
       </c>
       <c r="E16">
-        <v>27.428000000000001</v>
+        <v>2.7427999999999999</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -820,10 +831,10 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>106.307</v>
+        <v>10.630700000000001</v>
       </c>
       <c r="E17">
-        <v>25.456</v>
+        <v>2.5455999999999999</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -843,10 +854,10 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>91.823999999999998</v>
+        <v>9.1823999999999995</v>
       </c>
       <c r="E18">
-        <v>10.973000000000001</v>
+        <v>1.0973000000000002</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -866,10 +877,10 @@
         <v>3</v>
       </c>
       <c r="D19">
-        <v>98.272999999999996</v>
+        <v>9.8272999999999993</v>
       </c>
       <c r="E19">
-        <v>17.422000000000001</v>
+        <v>1.7422</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -889,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>100.995</v>
+        <v>10.099500000000001</v>
       </c>
       <c r="E20">
-        <v>25.263999999999999</v>
+        <v>2.5263999999999998</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -912,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>111.17749999999999</v>
+        <v>11.117749999999999</v>
       </c>
       <c r="E21">
-        <v>35.4465</v>
+        <v>3.5446499999999999</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -935,10 +946,10 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>109.5595</v>
+        <v>10.95595</v>
       </c>
       <c r="E22">
-        <v>33.828499999999998</v>
+        <v>3.3828499999999999</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -958,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>111.94750000000001</v>
+        <v>11.194750000000001</v>
       </c>
       <c r="E23">
-        <v>31.096499999999999</v>
+        <v>3.1096499999999998</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -981,10 +992,10 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>119.4765</v>
+        <v>11.947649999999999</v>
       </c>
       <c r="E24">
-        <v>38.625500000000002</v>
+        <v>3.8625500000000001</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1004,10 +1015,10 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <v>134.92099999999999</v>
+        <v>13.492099999999999</v>
       </c>
       <c r="E25">
-        <v>54.07</v>
+        <v>5.407</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1027,10 +1038,10 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>99.563500000000005</v>
+        <v>9.9563500000000005</v>
       </c>
       <c r="E26">
-        <v>23.8325</v>
+        <v>2.3832499999999999</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1050,10 +1061,10 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>109.629</v>
+        <v>10.962900000000001</v>
       </c>
       <c r="E27">
-        <v>33.898000000000003</v>
+        <v>3.3898000000000001</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1073,10 +1084,10 @@
         <v>3</v>
       </c>
       <c r="D28">
-        <v>109.485</v>
+        <v>10.948499999999999</v>
       </c>
       <c r="E28">
-        <v>33.753999999999998</v>
+        <v>3.3754</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1096,10 +1107,10 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>87.852999999999994</v>
+        <v>8.7852999999999994</v>
       </c>
       <c r="E29">
-        <v>7.0020000000000104</v>
+        <v>0.70020000000000104</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1119,10 +1130,10 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>98.345500000000001</v>
+        <v>9.8345500000000001</v>
       </c>
       <c r="E30">
-        <v>17.494499999999999</v>
+        <v>1.7494499999999999</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1142,10 +1153,10 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>92.93</v>
+        <v>9.293000000000001</v>
       </c>
       <c r="E31">
-        <v>12.079000000000001</v>
+        <v>1.2079</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1165,10 +1176,10 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>94.838499999999996</v>
+        <v>9.4838500000000003</v>
       </c>
       <c r="E32">
-        <v>19.107500000000002</v>
+        <v>1.9107500000000002</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1188,10 +1199,10 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>107.1735</v>
+        <v>10.71735</v>
       </c>
       <c r="E33">
-        <v>31.442499999999999</v>
+        <v>3.14425</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1211,10 +1222,10 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>106.726</v>
+        <v>10.672599999999999</v>
       </c>
       <c r="E34">
-        <v>30.995000000000001</v>
+        <v>3.0994999999999999</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1234,10 +1245,10 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>107.4515</v>
+        <v>10.745149999999999</v>
       </c>
       <c r="E35">
-        <v>26.6005</v>
+        <v>2.66005</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1257,10 +1268,10 @@
         <v>2</v>
       </c>
       <c r="D36">
-        <v>111.2825</v>
+        <v>11.12825</v>
       </c>
       <c r="E36">
-        <v>30.4315</v>
+        <v>3.0431499999999998</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1280,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="D37">
-        <v>108.066</v>
+        <v>10.8066</v>
       </c>
       <c r="E37">
-        <v>27.215</v>
+        <v>2.7214999999999998</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1303,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>83.908500000000004</v>
+        <v>8.3908500000000004</v>
       </c>
       <c r="E38">
-        <v>8.1775000000000109</v>
+        <v>0.81775000000000109</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1326,10 +1337,10 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>77.886499999999998</v>
+        <v>7.7886499999999996</v>
       </c>
       <c r="E39">
-        <v>2.15550000000002</v>
+        <v>0.21555000000000199</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1349,10 +1360,10 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <v>78.162000000000006</v>
+        <v>7.8162000000000003</v>
       </c>
       <c r="E40">
-        <v>2.4310000000000098</v>
+        <v>0.24310000000000098</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1372,10 +1383,10 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>89.138499999999993</v>
+        <v>8.9138500000000001</v>
       </c>
       <c r="E41">
-        <v>8.2874999999999908</v>
+        <v>0.8287499999999991</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1395,10 +1406,10 @@
         <v>2</v>
       </c>
       <c r="D42">
-        <v>81.939499999999995</v>
+        <v>8.1939499999999992</v>
       </c>
       <c r="E42">
-        <v>1.0885</v>
+        <v>0.10885</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1418,10 +1429,10 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <v>79.408500000000004</v>
+        <v>7.9408500000000002</v>
       </c>
       <c r="E43">
-        <v>-1.4424999999999999</v>
+        <v>-0.14424999999999999</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1441,10 +1452,10 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>108.4145</v>
+        <v>10.84145</v>
       </c>
       <c r="E44">
-        <v>32.683500000000002</v>
+        <v>3.2683500000000003</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1464,10 +1475,10 @@
         <v>2</v>
       </c>
       <c r="D45">
-        <v>110.124</v>
+        <v>11.0124</v>
       </c>
       <c r="E45">
-        <v>34.393000000000001</v>
+        <v>3.4393000000000002</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1487,10 +1498,10 @@
         <v>3</v>
       </c>
       <c r="D46">
-        <v>104.3925</v>
+        <v>10.439249999999999</v>
       </c>
       <c r="E46">
-        <v>28.6615</v>
+        <v>2.8661500000000002</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1510,10 +1521,10 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>108.748</v>
+        <v>10.8748</v>
       </c>
       <c r="E47">
-        <v>27.896999999999998</v>
+        <v>2.7896999999999998</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1533,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>108.3325</v>
+        <v>10.83325</v>
       </c>
       <c r="E48">
-        <v>27.4815</v>
+        <v>2.7481499999999999</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1556,10 +1567,10 @@
         <v>3</v>
       </c>
       <c r="D49">
-        <v>107.7105</v>
+        <v>10.771049999999999</v>
       </c>
       <c r="E49">
-        <v>26.859500000000001</v>
+        <v>2.6859500000000001</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -1579,10 +1590,10 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>104.187</v>
+        <v>10.418699999999999</v>
       </c>
       <c r="E50">
-        <v>28.456</v>
+        <v>2.8456000000000001</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1602,10 +1613,10 @@
         <v>2</v>
       </c>
       <c r="D51">
-        <v>107.9235</v>
+        <v>10.792350000000001</v>
       </c>
       <c r="E51">
-        <v>32.192500000000003</v>
+        <v>3.2192500000000002</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -1625,10 +1636,10 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <v>99.259500000000003</v>
+        <v>9.9259500000000003</v>
       </c>
       <c r="E52">
-        <v>23.528500000000001</v>
+        <v>2.3528500000000001</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1648,10 +1659,10 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>101.1795</v>
+        <v>10.11795</v>
       </c>
       <c r="E53">
-        <v>20.328499999999998</v>
+        <v>2.0328499999999998</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -1671,10 +1682,10 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>100.0515</v>
+        <v>10.00515</v>
       </c>
       <c r="E54">
-        <v>19.200500000000002</v>
+        <v>1.9200500000000003</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -1694,10 +1705,10 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <v>92.308499999999995</v>
+        <v>9.2308500000000002</v>
       </c>
       <c r="E55">
-        <v>11.4575</v>
+        <v>1.14575</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -1717,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>79.616500000000002</v>
+        <v>7.9616500000000006</v>
       </c>
       <c r="E56">
-        <v>3.8855000000000102</v>
+        <v>0.38855000000000101</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1740,10 +1751,10 @@
         <v>2</v>
       </c>
       <c r="D57">
-        <v>80.983000000000004</v>
+        <v>8.0983000000000001</v>
       </c>
       <c r="E57">
-        <v>5.2520000000000104</v>
+        <v>0.525200000000001</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -1763,10 +1774,10 @@
         <v>3</v>
       </c>
       <c r="D58">
-        <v>79.358999999999995</v>
+        <v>7.9358999999999993</v>
       </c>
       <c r="E58">
-        <v>3.6280000000000001</v>
+        <v>0.36280000000000001</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1786,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>80.490499999999997</v>
+        <v>8.0490499999999994</v>
       </c>
       <c r="E59">
-        <v>-0.36050000000000199</v>
+        <v>-3.60500000000002E-2</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -1809,10 +1820,10 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <v>87.3155</v>
+        <v>8.7315500000000004</v>
       </c>
       <c r="E60">
-        <v>6.4645000000000001</v>
+        <v>0.64644999999999997</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1832,10 +1843,10 @@
         <v>3</v>
       </c>
       <c r="D61">
-        <v>89.332499999999996</v>
+        <v>8.9332499999999992</v>
       </c>
       <c r="E61">
-        <v>8.4815000000000094</v>
+        <v>0.84815000000000096</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -1855,10 +1866,10 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>187.19988888888901</v>
+        <v>18.719988888888899</v>
       </c>
       <c r="E62">
-        <v>111.668888888889</v>
+        <v>11.1668888888889</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -1878,10 +1889,10 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>177.66311111111099</v>
+        <v>17.766311111111101</v>
       </c>
       <c r="E63">
-        <v>102.132111111111</v>
+        <v>10.2132111111111</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -1901,10 +1912,10 @@
         <v>3</v>
       </c>
       <c r="D64">
-        <v>176.31677777777799</v>
+        <v>17.631677777777799</v>
       </c>
       <c r="E64">
-        <v>100.78577777777799</v>
+        <v>10.078577777777799</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -1924,10 +1935,10 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>148.32599999999999</v>
+        <v>14.832599999999999</v>
       </c>
       <c r="E65">
-        <v>69.930999999999997</v>
+        <v>6.9931000000000001</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -1947,10 +1958,10 @@
         <v>2</v>
       </c>
       <c r="D66">
-        <v>143.024</v>
+        <v>14.3024</v>
       </c>
       <c r="E66">
-        <v>64.629000000000005</v>
+        <v>6.4629000000000003</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -1970,10 +1981,10 @@
         <v>3</v>
       </c>
       <c r="D67">
-        <v>148.10900000000001</v>
+        <v>14.8109</v>
       </c>
       <c r="E67">
-        <v>69.713999999999999</v>
+        <v>6.9714</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -1993,10 +2004,10 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>129.262</v>
+        <v>12.9262</v>
       </c>
       <c r="E68">
-        <v>53.731000000000002</v>
+        <v>5.3731</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2016,10 +2027,10 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>127.229</v>
+        <v>12.722899999999999</v>
       </c>
       <c r="E69">
-        <v>51.698</v>
+        <v>5.1698000000000004</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2039,10 +2050,10 @@
         <v>3</v>
       </c>
       <c r="D70">
-        <v>133.22</v>
+        <v>13.321999999999999</v>
       </c>
       <c r="E70">
-        <v>57.689</v>
+        <v>5.7689000000000004</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2062,10 +2073,10 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>131.07650000000001</v>
+        <v>13.107650000000001</v>
       </c>
       <c r="E71">
-        <v>52.6815</v>
+        <v>5.2681500000000003</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2085,10 +2096,10 @@
         <v>2</v>
       </c>
       <c r="D72">
-        <v>116.7435</v>
+        <v>11.67435</v>
       </c>
       <c r="E72">
-        <v>38.348500000000001</v>
+        <v>3.8348500000000003</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -2108,10 +2119,10 @@
         <v>3</v>
       </c>
       <c r="D73">
-        <v>131.0575</v>
+        <v>13.10575</v>
       </c>
       <c r="E73">
-        <v>52.662500000000001</v>
+        <v>5.2662500000000003</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -2131,10 +2142,10 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>134.506</v>
+        <v>13.4506</v>
       </c>
       <c r="E74">
-        <v>58.975000000000001</v>
+        <v>5.8975</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2154,10 +2165,10 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>137.839</v>
+        <v>13.783899999999999</v>
       </c>
       <c r="E75">
-        <v>62.308</v>
+        <v>6.2308000000000003</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2177,10 +2188,10 @@
         <v>3</v>
       </c>
       <c r="D76">
-        <v>140.5805</v>
+        <v>14.05805</v>
       </c>
       <c r="E76">
-        <v>65.049499999999995</v>
+        <v>6.5049499999999991</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2200,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <v>145.64599999999999</v>
+        <v>14.564599999999999</v>
       </c>
       <c r="E77">
-        <v>67.251000000000005</v>
+        <v>6.7251000000000003</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -2223,10 +2234,10 @@
         <v>2</v>
       </c>
       <c r="D78">
-        <v>138.4495</v>
+        <v>13.844950000000001</v>
       </c>
       <c r="E78">
-        <v>60.054499999999997</v>
+        <v>6.0054499999999997</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -2246,10 +2257,10 @@
         <v>3</v>
       </c>
       <c r="D79">
-        <v>144.6395</v>
+        <v>14.463950000000001</v>
       </c>
       <c r="E79">
-        <v>66.244500000000002</v>
+        <v>6.6244500000000004</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -2269,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>149.26249999999999</v>
+        <v>14.92625</v>
       </c>
       <c r="E80">
-        <v>73.731499999999997</v>
+        <v>7.3731499999999999</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2292,10 +2303,10 @@
         <v>2</v>
       </c>
       <c r="D81">
-        <v>151.37100000000001</v>
+        <v>15.1371</v>
       </c>
       <c r="E81">
-        <v>75.84</v>
+        <v>7.5840000000000005</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2315,10 +2326,10 @@
         <v>3</v>
       </c>
       <c r="D82">
-        <v>150.0625</v>
+        <v>15.00625</v>
       </c>
       <c r="E82">
-        <v>74.531499999999994</v>
+        <v>7.4531499999999991</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2338,10 +2349,10 @@
         <v>1</v>
       </c>
       <c r="D83">
-        <v>143.797</v>
+        <v>14.3797</v>
       </c>
       <c r="E83">
-        <v>65.402000000000001</v>
+        <v>6.5402000000000005</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -2361,10 +2372,10 @@
         <v>2</v>
       </c>
       <c r="D84">
-        <v>142.13200000000001</v>
+        <v>14.213200000000001</v>
       </c>
       <c r="E84">
-        <v>63.737000000000002</v>
+        <v>6.3737000000000004</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -2384,10 +2395,10 @@
         <v>3</v>
       </c>
       <c r="D85">
-        <v>141.16650000000001</v>
+        <v>14.116650000000002</v>
       </c>
       <c r="E85">
-        <v>62.771500000000003</v>
+        <v>6.2771500000000007</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -2407,10 +2418,10 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <v>146.1575</v>
+        <v>14.61575</v>
       </c>
       <c r="E86">
-        <v>70.626499999999993</v>
+        <v>7.0626499999999997</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -2430,10 +2441,10 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>159.61250000000001</v>
+        <v>15.961250000000001</v>
       </c>
       <c r="E87">
-        <v>84.081500000000005</v>
+        <v>8.4081500000000009</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -2453,10 +2464,10 @@
         <v>3</v>
       </c>
       <c r="D88">
-        <v>150.89250000000001</v>
+        <v>15.089250000000002</v>
       </c>
       <c r="E88">
-        <v>75.361500000000007</v>
+        <v>7.536150000000001</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -2476,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>143.65899999999999</v>
+        <v>14.3659</v>
       </c>
       <c r="E89">
-        <v>65.263999999999996</v>
+        <v>6.5263999999999998</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -2499,10 +2510,10 @@
         <v>2</v>
       </c>
       <c r="D90">
-        <v>147.67449999999999</v>
+        <v>14.76745</v>
       </c>
       <c r="E90">
-        <v>69.279499999999999</v>
+        <v>6.9279500000000001</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -2522,10 +2533,10 @@
         <v>3</v>
       </c>
       <c r="D91">
-        <v>153.68100000000001</v>
+        <v>15.368100000000002</v>
       </c>
       <c r="E91">
-        <v>75.286000000000001</v>
+        <v>7.5286</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -2545,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>158.137</v>
+        <v>15.813700000000001</v>
       </c>
       <c r="E92">
-        <v>82.605999999999995</v>
+        <v>8.2606000000000002</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -2568,10 +2579,10 @@
         <v>2</v>
       </c>
       <c r="D93">
-        <v>226.87649999999999</v>
+        <v>22.687649999999998</v>
       </c>
       <c r="E93">
-        <v>151.34549999999999</v>
+        <v>15.134549999999999</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2591,10 +2602,10 @@
         <v>3</v>
       </c>
       <c r="D94">
-        <v>149.61600000000001</v>
+        <v>14.961600000000001</v>
       </c>
       <c r="E94">
-        <v>74.084999999999994</v>
+        <v>7.4084999999999992</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -2614,10 +2625,10 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>159.21600000000001</v>
+        <v>15.921600000000002</v>
       </c>
       <c r="E95">
-        <v>80.820999999999998</v>
+        <v>8.0821000000000005</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -2637,10 +2648,10 @@
         <v>2</v>
       </c>
       <c r="D96">
-        <v>158.1875</v>
+        <v>15.81875</v>
       </c>
       <c r="E96">
-        <v>79.792500000000004</v>
+        <v>7.9792500000000004</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -2660,10 +2671,10 @@
         <v>3</v>
       </c>
       <c r="D97">
-        <v>172.54599999999999</v>
+        <v>17.2546</v>
       </c>
       <c r="E97">
-        <v>94.150999999999996</v>
+        <v>9.4150999999999989</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -2683,10 +2694,10 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <v>125.98050000000001</v>
+        <v>12.598050000000001</v>
       </c>
       <c r="E98">
-        <v>50.4495</v>
+        <v>5.04495</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -2706,10 +2717,10 @@
         <v>2</v>
       </c>
       <c r="D99">
-        <v>120.95950000000001</v>
+        <v>12.09595</v>
       </c>
       <c r="E99">
-        <v>45.4285</v>
+        <v>4.5428499999999996</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -2729,10 +2740,10 @@
         <v>3</v>
       </c>
       <c r="D100">
-        <v>124.3955</v>
+        <v>12.439550000000001</v>
       </c>
       <c r="E100">
-        <v>48.8645</v>
+        <v>4.88645</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -2752,10 +2763,10 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <v>117.4075</v>
+        <v>11.74075</v>
       </c>
       <c r="E101">
-        <v>39.012500000000003</v>
+        <v>3.9012500000000001</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -2775,10 +2786,10 @@
         <v>2</v>
       </c>
       <c r="D102">
-        <v>124.557</v>
+        <v>12.4557</v>
       </c>
       <c r="E102">
-        <v>46.161999999999999</v>
+        <v>4.6162000000000001</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -2798,10 +2809,10 @@
         <v>3</v>
       </c>
       <c r="D103">
-        <v>107.1365</v>
+        <v>10.713649999999999</v>
       </c>
       <c r="E103">
-        <v>28.741499999999998</v>
+        <v>2.8741499999999998</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -2821,10 +2832,10 @@
         <v>1</v>
       </c>
       <c r="D104">
-        <v>147.6395</v>
+        <v>14.763949999999999</v>
       </c>
       <c r="E104">
-        <v>72.108500000000006</v>
+        <v>7.2108500000000006</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -2844,10 +2855,10 @@
         <v>2</v>
       </c>
       <c r="D105">
-        <v>153.10149999999999</v>
+        <v>15.310149999999998</v>
       </c>
       <c r="E105">
-        <v>77.570499999999996</v>
+        <v>7.7570499999999996</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -2867,10 +2878,10 @@
         <v>3</v>
       </c>
       <c r="D106">
-        <v>140.44399999999999</v>
+        <v>14.0444</v>
       </c>
       <c r="E106">
-        <v>64.912999999999997</v>
+        <v>6.4912999999999998</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -2890,10 +2901,10 @@
         <v>1</v>
       </c>
       <c r="D107">
-        <v>144.2525</v>
+        <v>14.42525</v>
       </c>
       <c r="E107">
-        <v>65.857500000000002</v>
+        <v>6.58575</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -2913,10 +2924,10 @@
         <v>2</v>
       </c>
       <c r="D108">
-        <v>155.27449999999999</v>
+        <v>15.527449999999998</v>
       </c>
       <c r="E108">
-        <v>76.879499999999993</v>
+        <v>7.687949999999999</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -2936,10 +2947,10 @@
         <v>3</v>
       </c>
       <c r="D109">
-        <v>149.9385</v>
+        <v>14.99385</v>
       </c>
       <c r="E109">
-        <v>71.543499999999995</v>
+        <v>7.1543499999999991</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -2959,10 +2970,10 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>171.767</v>
+        <v>17.1767</v>
       </c>
       <c r="E110">
-        <v>96.236000000000004</v>
+        <v>9.6235999999999997</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -2982,10 +2993,10 @@
         <v>2</v>
       </c>
       <c r="D111">
-        <v>199.2535</v>
+        <v>19.925350000000002</v>
       </c>
       <c r="E111">
-        <v>123.7225</v>
+        <v>12.372249999999999</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -3005,10 +3016,10 @@
         <v>3</v>
       </c>
       <c r="D112">
-        <v>186.61099999999999</v>
+        <v>18.661099999999998</v>
       </c>
       <c r="E112">
-        <v>111.08</v>
+        <v>11.108000000000001</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -3028,10 +3039,10 @@
         <v>1</v>
       </c>
       <c r="D113">
-        <v>145.685</v>
+        <v>14.5685</v>
       </c>
       <c r="E113">
-        <v>67.290000000000006</v>
+        <v>6.729000000000001</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -3051,10 +3062,10 @@
         <v>2</v>
       </c>
       <c r="D114">
-        <v>171.85849999999999</v>
+        <v>17.185849999999999</v>
       </c>
       <c r="E114">
-        <v>93.463499999999996</v>
+        <v>9.3463499999999993</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -3074,10 +3085,10 @@
         <v>3</v>
       </c>
       <c r="D115">
-        <v>149.54750000000001</v>
+        <v>14.954750000000001</v>
       </c>
       <c r="E115">
-        <v>71.152500000000003</v>
+        <v>7.1152500000000005</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -3097,10 +3108,10 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>81.782499999999999</v>
+        <v>8.1782500000000002</v>
       </c>
       <c r="E116">
-        <v>6.2514999999999903</v>
+        <v>0.62514999999999898</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -3120,10 +3131,10 @@
         <v>2</v>
       </c>
       <c r="D117">
-        <v>81.867000000000004</v>
+        <v>8.1867000000000001</v>
       </c>
       <c r="E117">
-        <v>6.3359999999999799</v>
+        <v>0.63359999999999794</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -3143,10 +3154,10 @@
         <v>3</v>
       </c>
       <c r="D118">
-        <v>82.843000000000004</v>
+        <v>8.2843</v>
       </c>
       <c r="E118">
-        <v>7.3119999999999798</v>
+        <v>0.73119999999999796</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -3166,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="D119">
-        <v>124.91249999999999</v>
+        <v>12.491249999999999</v>
       </c>
       <c r="E119">
-        <v>46.517499999999998</v>
+        <v>4.6517499999999998</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -3189,10 +3200,10 @@
         <v>2</v>
       </c>
       <c r="D120">
-        <v>124.375</v>
+        <v>12.4375</v>
       </c>
       <c r="E120">
-        <v>45.98</v>
+        <v>4.5979999999999999</v>
       </c>
       <c r="F120">
         <v>0</v>
@@ -3212,10 +3223,10 @@
         <v>3</v>
       </c>
       <c r="D121">
-        <v>127.4915</v>
+        <v>12.74915</v>
       </c>
       <c r="E121">
-        <v>49.096499999999999</v>
+        <v>4.9096500000000001</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -3225,7 +3236,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G121">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G121">
     <sortCondition ref="G2:G121"/>
     <sortCondition ref="A2:A121"/>
   </sortState>

</xml_diff>